<commit_message>
Implement image display in question text
</commit_message>
<xml_diff>
--- a/www/anatomy.xlsx
+++ b/www/anatomy.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Data/Clients/r/reviseR/www/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AECA54E-2EAC-7A42-A2DA-760CA7E45509}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A74CCC83-F440-5742-8E92-25002DC77704}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30800" yWindow="2020" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{75AEF49E-9248-134F-BD7C-8C840DEAD4B8}"/>
+    <workbookView xWindow="3180" yWindow="2360" windowWidth="28040" windowHeight="17440" xr2:uid="{75AEF49E-9248-134F-BD7C-8C840DEAD4B8}"/>
   </bookViews>
   <sheets>
     <sheet name="Questions" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="558" uniqueCount="157">
   <si>
     <t>Category</t>
   </si>
@@ -434,6 +434,78 @@
   </si>
   <si>
     <t>relating to the jaw</t>
+  </si>
+  <si>
+    <t>Bone is composed of two types of tissue called</t>
+  </si>
+  <si>
+    <t>Compact and cancellous</t>
+  </si>
+  <si>
+    <t>Compact and loose</t>
+  </si>
+  <si>
+    <t>Lamellae and canaliculi</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>The periosteum</t>
+  </si>
+  <si>
+    <t>The cancellous</t>
+  </si>
+  <si>
+    <t>Ligament</t>
+  </si>
+  <si>
+    <t>The fibrous membrane almost surrounding bones is called</t>
+  </si>
+  <si>
+    <t>At joints, bones are covered by</t>
+  </si>
+  <si>
+    <t>Hyaline cartilage</t>
+  </si>
+  <si>
+    <t>Lyaline cartilage</t>
+  </si>
+  <si>
+    <t>Ligaments</t>
+  </si>
+  <si>
+    <t>Tendons</t>
+  </si>
+  <si>
+    <t>The periosteum has a rich blood supply, hyaline cartilage has a poor blood supply</t>
+  </si>
+  <si>
+    <t>The periosteum has a poor blood supply, hyaline cartilage has a rich blood supply</t>
+  </si>
+  <si>
+    <t>Both the periosteum and hyaline catilage have a rich blood supply</t>
+  </si>
+  <si>
+    <t>Both the periosteum and hyaline catilage have a poor blood supply</t>
+  </si>
+  <si>
+    <t>Which of the following statements is true?</t>
+  </si>
+  <si>
+    <t>Protects bone</t>
+  </si>
+  <si>
+    <t>Has a poor blood supply</t>
+  </si>
+  <si>
+    <t>Is the site of attachment of ligaments and tendons</t>
+  </si>
+  <si>
+    <t>Is the site of bone growth</t>
+  </si>
+  <si>
+    <t>Definitions</t>
   </si>
 </sst>
 </file>
@@ -810,10 +882,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D8A4190-821E-5141-8EE6-FFBFC191691E}">
-  <dimension ref="A1:G32"/>
+  <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26:B32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -942,7 +1015,7 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>30</v>
+        <v>156</v>
       </c>
       <c r="C8">
         <v>7</v>
@@ -956,7 +1029,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>30</v>
+        <v>156</v>
       </c>
       <c r="C9">
         <v>8</v>
@@ -970,7 +1043,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>30</v>
+        <v>156</v>
       </c>
       <c r="C10">
         <v>9</v>
@@ -984,7 +1057,7 @@
         <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>30</v>
+        <v>156</v>
       </c>
       <c r="C11">
         <v>10</v>
@@ -997,8 +1070,8 @@
       <c r="A12" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="4" t="s">
-        <v>30</v>
+      <c r="B12" t="s">
+        <v>156</v>
       </c>
       <c r="C12">
         <v>11</v>
@@ -1011,8 +1084,8 @@
       <c r="A13" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="4" t="s">
-        <v>30</v>
+      <c r="B13" t="s">
+        <v>156</v>
       </c>
       <c r="C13">
         <v>12</v>
@@ -1025,8 +1098,8 @@
       <c r="A14" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="4" t="s">
-        <v>30</v>
+      <c r="B14" t="s">
+        <v>156</v>
       </c>
       <c r="C14">
         <v>13</v>
@@ -1039,8 +1112,8 @@
       <c r="A15" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B15" s="4" t="s">
-        <v>30</v>
+      <c r="B15" t="s">
+        <v>156</v>
       </c>
       <c r="C15">
         <v>14</v>
@@ -1053,8 +1126,8 @@
       <c r="A16" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="4" t="s">
-        <v>30</v>
+      <c r="B16" t="s">
+        <v>156</v>
       </c>
       <c r="C16">
         <v>15</v>
@@ -1067,8 +1140,8 @@
       <c r="A17" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B17" s="4" t="s">
-        <v>30</v>
+      <c r="B17" t="s">
+        <v>156</v>
       </c>
       <c r="C17">
         <v>16</v>
@@ -1081,8 +1154,8 @@
       <c r="A18" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B18" s="4" t="s">
-        <v>30</v>
+      <c r="B18" t="s">
+        <v>156</v>
       </c>
       <c r="C18">
         <v>17</v>
@@ -1095,8 +1168,8 @@
       <c r="A19" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B19" s="4" t="s">
-        <v>30</v>
+      <c r="B19" t="s">
+        <v>156</v>
       </c>
       <c r="C19">
         <v>18</v>
@@ -1109,8 +1182,8 @@
       <c r="A20" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B20" s="4" t="s">
-        <v>30</v>
+      <c r="B20" t="s">
+        <v>156</v>
       </c>
       <c r="C20">
         <v>19</v>
@@ -1123,8 +1196,8 @@
       <c r="A21" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B21" s="4" t="s">
-        <v>30</v>
+      <c r="B21" t="s">
+        <v>156</v>
       </c>
       <c r="C21">
         <v>20</v>
@@ -1137,8 +1210,8 @@
       <c r="A22" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B22" s="4" t="s">
-        <v>30</v>
+      <c r="B22" t="s">
+        <v>156</v>
       </c>
       <c r="C22">
         <v>21</v>
@@ -1151,8 +1224,8 @@
       <c r="A23" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B23" s="4" t="s">
-        <v>30</v>
+      <c r="B23" t="s">
+        <v>156</v>
       </c>
       <c r="C23">
         <v>22</v>
@@ -1165,8 +1238,8 @@
       <c r="A24" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B24" s="4" t="s">
-        <v>30</v>
+      <c r="B24" t="s">
+        <v>156</v>
       </c>
       <c r="C24">
         <v>23</v>
@@ -1179,8 +1252,8 @@
       <c r="A25" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B25" s="4" t="s">
-        <v>30</v>
+      <c r="B25" t="s">
+        <v>156</v>
       </c>
       <c r="C25">
         <v>24</v>
@@ -1193,8 +1266,8 @@
       <c r="A26" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B26" s="4" t="s">
-        <v>30</v>
+      <c r="B26" t="s">
+        <v>156</v>
       </c>
       <c r="C26">
         <v>25</v>
@@ -1207,8 +1280,8 @@
       <c r="A27" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B27" s="4" t="s">
-        <v>30</v>
+      <c r="B27" t="s">
+        <v>156</v>
       </c>
       <c r="C27">
         <v>26</v>
@@ -1221,8 +1294,8 @@
       <c r="A28" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B28" s="4" t="s">
-        <v>30</v>
+      <c r="B28" t="s">
+        <v>156</v>
       </c>
       <c r="C28">
         <v>27</v>
@@ -1235,8 +1308,8 @@
       <c r="A29" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B29" s="4" t="s">
-        <v>30</v>
+      <c r="B29" t="s">
+        <v>156</v>
       </c>
       <c r="C29">
         <v>28</v>
@@ -1249,8 +1322,8 @@
       <c r="A30" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B30" s="4" t="s">
-        <v>30</v>
+      <c r="B30" t="s">
+        <v>156</v>
       </c>
       <c r="C30">
         <v>29</v>
@@ -1263,8 +1336,8 @@
       <c r="A31" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B31" s="4" t="s">
-        <v>30</v>
+      <c r="B31" t="s">
+        <v>156</v>
       </c>
       <c r="C31">
         <v>30</v>
@@ -1277,14 +1350,84 @@
       <c r="A32" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B32" s="4" t="s">
-        <v>30</v>
+      <c r="B32" t="s">
+        <v>156</v>
       </c>
       <c r="C32">
         <v>31</v>
       </c>
       <c r="D32" t="s">
         <v>128</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C33">
+        <v>32</v>
+      </c>
+      <c r="D33" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C34">
+        <v>33</v>
+      </c>
+      <c r="D34" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C35">
+        <v>34</v>
+      </c>
+      <c r="D35" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C36">
+        <v>35</v>
+      </c>
+      <c r="D36" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C37">
+        <v>36</v>
+      </c>
+      <c r="D37" t="s">
+        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -1294,11 +1437,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83DF9C1B-75A2-E34D-B3C5-7E9DE5A0F39E}">
-  <dimension ref="A1:G119"/>
+  <dimension ref="A1:G138"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F119" sqref="F119"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A106" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D120" sqref="D120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1703,7 +1846,7 @@
         <v>8</v>
       </c>
       <c r="B25" t="s">
-        <v>30</v>
+        <v>156</v>
       </c>
       <c r="C25">
         <v>7</v>
@@ -1720,7 +1863,7 @@
         <v>8</v>
       </c>
       <c r="B26" t="s">
-        <v>30</v>
+        <v>156</v>
       </c>
       <c r="C26">
         <v>7</v>
@@ -1734,7 +1877,7 @@
         <v>8</v>
       </c>
       <c r="B27" t="s">
-        <v>30</v>
+        <v>156</v>
       </c>
       <c r="C27">
         <v>7</v>
@@ -1748,7 +1891,7 @@
         <v>8</v>
       </c>
       <c r="B28" t="s">
-        <v>30</v>
+        <v>156</v>
       </c>
       <c r="C28">
         <v>7</v>
@@ -1762,7 +1905,7 @@
         <v>8</v>
       </c>
       <c r="B29" t="s">
-        <v>30</v>
+        <v>156</v>
       </c>
       <c r="C29">
         <v>8</v>
@@ -1776,7 +1919,7 @@
         <v>8</v>
       </c>
       <c r="B30" t="s">
-        <v>30</v>
+        <v>156</v>
       </c>
       <c r="C30">
         <v>8</v>
@@ -1793,7 +1936,7 @@
         <v>8</v>
       </c>
       <c r="B31" t="s">
-        <v>30</v>
+        <v>156</v>
       </c>
       <c r="C31">
         <v>8</v>
@@ -1807,7 +1950,7 @@
         <v>8</v>
       </c>
       <c r="B32" t="s">
-        <v>30</v>
+        <v>156</v>
       </c>
       <c r="C32">
         <v>8</v>
@@ -1820,8 +1963,8 @@
       <c r="A33" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B33" s="4" t="s">
-        <v>30</v>
+      <c r="B33" t="s">
+        <v>156</v>
       </c>
       <c r="C33" s="4">
         <v>9</v>
@@ -1835,8 +1978,8 @@
       <c r="A34" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B34" s="4" t="s">
-        <v>30</v>
+      <c r="B34" t="s">
+        <v>156</v>
       </c>
       <c r="C34" s="4">
         <v>9</v>
@@ -1850,8 +1993,8 @@
       <c r="A35" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B35" s="4" t="s">
-        <v>30</v>
+      <c r="B35" t="s">
+        <v>156</v>
       </c>
       <c r="C35" s="4">
         <v>9</v>
@@ -1868,8 +2011,8 @@
       <c r="A36" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B36" s="4" t="s">
-        <v>30</v>
+      <c r="B36" t="s">
+        <v>156</v>
       </c>
       <c r="C36" s="4">
         <v>10</v>
@@ -1885,8 +2028,8 @@
       <c r="A37" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B37" s="4" t="s">
-        <v>30</v>
+      <c r="B37" t="s">
+        <v>156</v>
       </c>
       <c r="C37" s="4">
         <v>10</v>
@@ -1899,8 +2042,8 @@
       <c r="A38" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B38" s="4" t="s">
-        <v>30</v>
+      <c r="B38" t="s">
+        <v>156</v>
       </c>
       <c r="C38" s="4">
         <v>10</v>
@@ -1913,8 +2056,8 @@
       <c r="A39" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B39" s="4" t="s">
-        <v>30</v>
+      <c r="B39" t="s">
+        <v>156</v>
       </c>
       <c r="C39" s="4">
         <v>10</v>
@@ -1927,8 +2070,8 @@
       <c r="A40" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B40" s="4" t="s">
-        <v>30</v>
+      <c r="B40" t="s">
+        <v>156</v>
       </c>
       <c r="C40" s="4">
         <v>11</v>
@@ -1944,8 +2087,8 @@
       <c r="A41" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B41" s="4" t="s">
-        <v>30</v>
+      <c r="B41" t="s">
+        <v>156</v>
       </c>
       <c r="C41" s="4">
         <v>11</v>
@@ -1958,8 +2101,8 @@
       <c r="A42" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B42" s="4" t="s">
-        <v>30</v>
+      <c r="B42" t="s">
+        <v>156</v>
       </c>
       <c r="C42" s="4">
         <v>11</v>
@@ -1972,8 +2115,8 @@
       <c r="A43" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B43" s="4" t="s">
-        <v>30</v>
+      <c r="B43" t="s">
+        <v>156</v>
       </c>
       <c r="C43" s="4">
         <v>11</v>
@@ -1986,8 +2129,8 @@
       <c r="A44" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B44" s="4" t="s">
-        <v>30</v>
+      <c r="B44" t="s">
+        <v>156</v>
       </c>
       <c r="C44" s="4">
         <v>11</v>
@@ -2000,8 +2143,8 @@
       <c r="A45" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B45" s="4" t="s">
-        <v>30</v>
+      <c r="B45" t="s">
+        <v>156</v>
       </c>
       <c r="C45" s="4">
         <v>12</v>
@@ -2017,8 +2160,8 @@
       <c r="A46" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B46" s="4" t="s">
-        <v>30</v>
+      <c r="B46" t="s">
+        <v>156</v>
       </c>
       <c r="C46" s="4">
         <v>12</v>
@@ -2031,8 +2174,8 @@
       <c r="A47" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B47" s="4" t="s">
-        <v>30</v>
+      <c r="B47" t="s">
+        <v>156</v>
       </c>
       <c r="C47" s="4">
         <v>12</v>
@@ -2045,8 +2188,8 @@
       <c r="A48" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B48" s="4" t="s">
-        <v>30</v>
+      <c r="B48" t="s">
+        <v>156</v>
       </c>
       <c r="C48" s="4">
         <v>13</v>
@@ -2059,8 +2202,8 @@
       <c r="A49" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B49" s="4" t="s">
-        <v>30</v>
+      <c r="B49" t="s">
+        <v>156</v>
       </c>
       <c r="C49" s="4">
         <v>13</v>
@@ -2076,8 +2219,8 @@
       <c r="A50" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B50" s="4" t="s">
-        <v>30</v>
+      <c r="B50" t="s">
+        <v>156</v>
       </c>
       <c r="C50" s="4">
         <v>13</v>
@@ -2090,8 +2233,8 @@
       <c r="A51" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B51" s="4" t="s">
-        <v>30</v>
+      <c r="B51" t="s">
+        <v>156</v>
       </c>
       <c r="C51" s="4">
         <v>14</v>
@@ -2104,8 +2247,8 @@
       <c r="A52" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B52" s="4" t="s">
-        <v>30</v>
+      <c r="B52" t="s">
+        <v>156</v>
       </c>
       <c r="C52" s="4">
         <v>14</v>
@@ -2118,8 +2261,8 @@
       <c r="A53" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B53" s="4" t="s">
-        <v>30</v>
+      <c r="B53" t="s">
+        <v>156</v>
       </c>
       <c r="C53" s="4">
         <v>14</v>
@@ -2135,8 +2278,8 @@
       <c r="A54" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B54" s="4" t="s">
-        <v>30</v>
+      <c r="B54" t="s">
+        <v>156</v>
       </c>
       <c r="C54" s="4">
         <v>15</v>
@@ -2152,8 +2295,8 @@
       <c r="A55" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B55" s="4" t="s">
-        <v>30</v>
+      <c r="B55" t="s">
+        <v>156</v>
       </c>
       <c r="C55" s="4">
         <v>15</v>
@@ -2166,8 +2309,8 @@
       <c r="A56" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B56" s="4" t="s">
-        <v>30</v>
+      <c r="B56" t="s">
+        <v>156</v>
       </c>
       <c r="C56" s="4">
         <v>15</v>
@@ -2180,8 +2323,8 @@
       <c r="A57" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B57" s="4" t="s">
-        <v>30</v>
+      <c r="B57" t="s">
+        <v>156</v>
       </c>
       <c r="C57" s="4">
         <v>15</v>
@@ -2194,8 +2337,8 @@
       <c r="A58" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B58" s="4" t="s">
-        <v>30</v>
+      <c r="B58" t="s">
+        <v>156</v>
       </c>
       <c r="C58" s="4">
         <v>16</v>
@@ -2211,8 +2354,8 @@
       <c r="A59" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B59" s="4" t="s">
-        <v>30</v>
+      <c r="B59" t="s">
+        <v>156</v>
       </c>
       <c r="C59" s="4">
         <v>16</v>
@@ -2225,8 +2368,8 @@
       <c r="A60" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B60" s="4" t="s">
-        <v>30</v>
+      <c r="B60" t="s">
+        <v>156</v>
       </c>
       <c r="C60" s="4">
         <v>16</v>
@@ -2239,8 +2382,8 @@
       <c r="A61" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B61" s="4" t="s">
-        <v>30</v>
+      <c r="B61" t="s">
+        <v>156</v>
       </c>
       <c r="C61" s="4">
         <v>16</v>
@@ -2253,8 +2396,8 @@
       <c r="A62" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B62" s="4" t="s">
-        <v>30</v>
+      <c r="B62" t="s">
+        <v>156</v>
       </c>
       <c r="C62" s="4">
         <v>17</v>
@@ -2270,8 +2413,8 @@
       <c r="A63" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B63" s="4" t="s">
-        <v>30</v>
+      <c r="B63" t="s">
+        <v>156</v>
       </c>
       <c r="C63" s="4">
         <v>17</v>
@@ -2284,8 +2427,8 @@
       <c r="A64" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B64" s="4" t="s">
-        <v>30</v>
+      <c r="B64" t="s">
+        <v>156</v>
       </c>
       <c r="C64" s="4">
         <v>17</v>
@@ -2298,8 +2441,8 @@
       <c r="A65" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B65" s="4" t="s">
-        <v>30</v>
+      <c r="B65" t="s">
+        <v>156</v>
       </c>
       <c r="C65" s="4">
         <v>17</v>
@@ -2312,8 +2455,8 @@
       <c r="A66" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B66" s="4" t="s">
-        <v>30</v>
+      <c r="B66" t="s">
+        <v>156</v>
       </c>
       <c r="C66" s="4">
         <v>18</v>
@@ -2329,8 +2472,8 @@
       <c r="A67" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B67" s="4" t="s">
-        <v>30</v>
+      <c r="B67" t="s">
+        <v>156</v>
       </c>
       <c r="C67" s="4">
         <v>18</v>
@@ -2343,8 +2486,8 @@
       <c r="A68" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B68" s="4" t="s">
-        <v>30</v>
+      <c r="B68" t="s">
+        <v>156</v>
       </c>
       <c r="C68" s="4">
         <v>18</v>
@@ -2357,8 +2500,8 @@
       <c r="A69" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B69" s="4" t="s">
-        <v>30</v>
+      <c r="B69" t="s">
+        <v>156</v>
       </c>
       <c r="C69" s="4">
         <v>19</v>
@@ -2374,8 +2517,8 @@
       <c r="A70" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B70" s="4" t="s">
-        <v>30</v>
+      <c r="B70" t="s">
+        <v>156</v>
       </c>
       <c r="C70" s="4">
         <v>19</v>
@@ -2388,8 +2531,8 @@
       <c r="A71" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B71" s="4" t="s">
-        <v>30</v>
+      <c r="B71" t="s">
+        <v>156</v>
       </c>
       <c r="C71" s="4">
         <v>19</v>
@@ -2402,8 +2545,8 @@
       <c r="A72" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B72" s="4" t="s">
-        <v>30</v>
+      <c r="B72" t="s">
+        <v>156</v>
       </c>
       <c r="C72" s="4">
         <v>20</v>
@@ -2419,8 +2562,8 @@
       <c r="A73" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B73" s="4" t="s">
-        <v>30</v>
+      <c r="B73" t="s">
+        <v>156</v>
       </c>
       <c r="C73" s="4">
         <v>20</v>
@@ -2433,8 +2576,8 @@
       <c r="A74" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B74" s="4" t="s">
-        <v>30</v>
+      <c r="B74" t="s">
+        <v>156</v>
       </c>
       <c r="C74" s="4">
         <v>20</v>
@@ -2447,8 +2590,8 @@
       <c r="A75" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B75" s="4" t="s">
-        <v>30</v>
+      <c r="B75" t="s">
+        <v>156</v>
       </c>
       <c r="C75" s="4">
         <v>20</v>
@@ -2461,8 +2604,8 @@
       <c r="A76" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B76" s="4" t="s">
-        <v>30</v>
+      <c r="B76" t="s">
+        <v>156</v>
       </c>
       <c r="C76" s="4">
         <v>21</v>
@@ -2478,8 +2621,8 @@
       <c r="A77" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B77" s="4" t="s">
-        <v>30</v>
+      <c r="B77" t="s">
+        <v>156</v>
       </c>
       <c r="C77" s="4">
         <v>21</v>
@@ -2492,8 +2635,8 @@
       <c r="A78" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B78" s="4" t="s">
-        <v>30</v>
+      <c r="B78" t="s">
+        <v>156</v>
       </c>
       <c r="C78" s="4">
         <v>21</v>
@@ -2506,8 +2649,8 @@
       <c r="A79" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B79" s="4" t="s">
-        <v>30</v>
+      <c r="B79" t="s">
+        <v>156</v>
       </c>
       <c r="C79" s="4">
         <v>21</v>
@@ -2520,8 +2663,8 @@
       <c r="A80" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B80" s="4" t="s">
-        <v>30</v>
+      <c r="B80" t="s">
+        <v>156</v>
       </c>
       <c r="C80">
         <v>22</v>
@@ -2537,8 +2680,8 @@
       <c r="A81" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B81" s="4" t="s">
-        <v>30</v>
+      <c r="B81" t="s">
+        <v>156</v>
       </c>
       <c r="C81" s="4">
         <v>22</v>
@@ -2551,8 +2694,8 @@
       <c r="A82" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B82" s="4" t="s">
-        <v>30</v>
+      <c r="B82" t="s">
+        <v>156</v>
       </c>
       <c r="C82" s="4">
         <v>22</v>
@@ -2565,8 +2708,8 @@
       <c r="A83" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B83" s="4" t="s">
-        <v>30</v>
+      <c r="B83" t="s">
+        <v>156</v>
       </c>
       <c r="C83" s="4">
         <v>22</v>
@@ -2579,8 +2722,8 @@
       <c r="A84" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B84" s="4" t="s">
-        <v>30</v>
+      <c r="B84" t="s">
+        <v>156</v>
       </c>
       <c r="C84" s="4">
         <v>23</v>
@@ -2596,8 +2739,8 @@
       <c r="A85" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B85" s="4" t="s">
-        <v>30</v>
+      <c r="B85" t="s">
+        <v>156</v>
       </c>
       <c r="C85" s="4">
         <v>23</v>
@@ -2610,8 +2753,8 @@
       <c r="A86" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B86" s="4" t="s">
-        <v>30</v>
+      <c r="B86" t="s">
+        <v>156</v>
       </c>
       <c r="C86" s="4">
         <v>23</v>
@@ -2624,8 +2767,8 @@
       <c r="A87" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B87" s="4" t="s">
-        <v>30</v>
+      <c r="B87" t="s">
+        <v>156</v>
       </c>
       <c r="C87" s="4">
         <v>23</v>
@@ -2638,8 +2781,8 @@
       <c r="A88" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B88" s="4" t="s">
-        <v>30</v>
+      <c r="B88" t="s">
+        <v>156</v>
       </c>
       <c r="C88" s="4">
         <v>24</v>
@@ -2652,8 +2795,8 @@
       <c r="A89" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B89" s="4" t="s">
-        <v>30</v>
+      <c r="B89" t="s">
+        <v>156</v>
       </c>
       <c r="C89" s="4">
         <v>24</v>
@@ -2666,8 +2809,8 @@
       <c r="A90" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B90" s="4" t="s">
-        <v>30</v>
+      <c r="B90" t="s">
+        <v>156</v>
       </c>
       <c r="C90" s="4">
         <v>24</v>
@@ -2680,8 +2823,8 @@
       <c r="A91" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B91" s="4" t="s">
-        <v>30</v>
+      <c r="B91" t="s">
+        <v>156</v>
       </c>
       <c r="C91" s="4">
         <v>24</v>
@@ -2694,8 +2837,8 @@
       <c r="A92" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B92" s="4" t="s">
-        <v>30</v>
+      <c r="B92" t="s">
+        <v>156</v>
       </c>
       <c r="C92" s="4">
         <v>25</v>
@@ -2711,8 +2854,8 @@
       <c r="A93" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B93" s="4" t="s">
-        <v>30</v>
+      <c r="B93" t="s">
+        <v>156</v>
       </c>
       <c r="C93" s="4">
         <v>25</v>
@@ -2725,8 +2868,8 @@
       <c r="A94" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B94" s="4" t="s">
-        <v>30</v>
+      <c r="B94" t="s">
+        <v>156</v>
       </c>
       <c r="C94" s="4">
         <v>25</v>
@@ -2739,8 +2882,8 @@
       <c r="A95" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B95" s="4" t="s">
-        <v>30</v>
+      <c r="B95" t="s">
+        <v>156</v>
       </c>
       <c r="C95" s="4">
         <v>25</v>
@@ -2753,8 +2896,8 @@
       <c r="A96" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B96" s="4" t="s">
-        <v>30</v>
+      <c r="B96" t="s">
+        <v>156</v>
       </c>
       <c r="C96" s="4">
         <v>26</v>
@@ -2770,8 +2913,8 @@
       <c r="A97" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B97" s="4" t="s">
-        <v>30</v>
+      <c r="B97" t="s">
+        <v>156</v>
       </c>
       <c r="C97" s="4">
         <v>26</v>
@@ -2784,8 +2927,8 @@
       <c r="A98" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B98" s="4" t="s">
-        <v>30</v>
+      <c r="B98" t="s">
+        <v>156</v>
       </c>
       <c r="C98" s="4">
         <v>26</v>
@@ -2798,8 +2941,8 @@
       <c r="A99" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B99" s="4" t="s">
-        <v>30</v>
+      <c r="B99" t="s">
+        <v>156</v>
       </c>
       <c r="C99" s="4">
         <v>26</v>
@@ -2812,8 +2955,8 @@
       <c r="A100" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B100" s="4" t="s">
-        <v>30</v>
+      <c r="B100" t="s">
+        <v>156</v>
       </c>
       <c r="C100" s="4">
         <v>27</v>
@@ -2829,8 +2972,8 @@
       <c r="A101" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B101" s="4" t="s">
-        <v>30</v>
+      <c r="B101" t="s">
+        <v>156</v>
       </c>
       <c r="C101" s="4">
         <v>27</v>
@@ -2843,8 +2986,8 @@
       <c r="A102" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B102" s="4" t="s">
-        <v>30</v>
+      <c r="B102" t="s">
+        <v>156</v>
       </c>
       <c r="C102" s="4">
         <v>27</v>
@@ -2857,8 +3000,8 @@
       <c r="A103" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B103" s="4" t="s">
-        <v>30</v>
+      <c r="B103" t="s">
+        <v>156</v>
       </c>
       <c r="C103" s="4">
         <v>27</v>
@@ -2871,8 +3014,8 @@
       <c r="A104" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B104" s="4" t="s">
-        <v>30</v>
+      <c r="B104" t="s">
+        <v>156</v>
       </c>
       <c r="C104" s="4">
         <v>28</v>
@@ -2888,8 +3031,8 @@
       <c r="A105" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B105" s="4" t="s">
-        <v>30</v>
+      <c r="B105" t="s">
+        <v>156</v>
       </c>
       <c r="C105" s="4">
         <v>28</v>
@@ -2902,8 +3045,8 @@
       <c r="A106" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B106" s="4" t="s">
-        <v>30</v>
+      <c r="B106" t="s">
+        <v>156</v>
       </c>
       <c r="C106" s="4">
         <v>28</v>
@@ -2916,8 +3059,8 @@
       <c r="A107" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B107" s="4" t="s">
-        <v>30</v>
+      <c r="B107" t="s">
+        <v>156</v>
       </c>
       <c r="C107" s="4">
         <v>28</v>
@@ -2930,8 +3073,8 @@
       <c r="A108" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B108" s="4" t="s">
-        <v>30</v>
+      <c r="B108" t="s">
+        <v>156</v>
       </c>
       <c r="C108" s="4">
         <v>29</v>
@@ -2947,8 +3090,8 @@
       <c r="A109" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B109" s="4" t="s">
-        <v>30</v>
+      <c r="B109" t="s">
+        <v>156</v>
       </c>
       <c r="C109" s="4">
         <v>29</v>
@@ -2961,8 +3104,8 @@
       <c r="A110" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B110" s="4" t="s">
-        <v>30</v>
+      <c r="B110" t="s">
+        <v>156</v>
       </c>
       <c r="C110" s="4">
         <v>29</v>
@@ -2975,8 +3118,8 @@
       <c r="A111" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B111" s="4" t="s">
-        <v>30</v>
+      <c r="B111" t="s">
+        <v>156</v>
       </c>
       <c r="C111" s="4">
         <v>29</v>
@@ -2989,8 +3132,8 @@
       <c r="A112" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B112" s="4" t="s">
-        <v>30</v>
+      <c r="B112" t="s">
+        <v>156</v>
       </c>
       <c r="C112" s="4">
         <v>30</v>
@@ -3006,8 +3149,8 @@
       <c r="A113" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B113" s="4" t="s">
-        <v>30</v>
+      <c r="B113" t="s">
+        <v>156</v>
       </c>
       <c r="C113" s="4">
         <v>30</v>
@@ -3020,8 +3163,8 @@
       <c r="A114" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B114" s="4" t="s">
-        <v>30</v>
+      <c r="B114" t="s">
+        <v>156</v>
       </c>
       <c r="C114" s="4">
         <v>30</v>
@@ -3034,8 +3177,8 @@
       <c r="A115" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B115" s="4" t="s">
-        <v>30</v>
+      <c r="B115" t="s">
+        <v>156</v>
       </c>
       <c r="C115" s="4">
         <v>30</v>
@@ -3048,8 +3191,8 @@
       <c r="A116" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B116" s="4" t="s">
-        <v>30</v>
+      <c r="B116" t="s">
+        <v>156</v>
       </c>
       <c r="C116" s="4">
         <v>31</v>
@@ -3065,8 +3208,8 @@
       <c r="A117" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B117" s="4" t="s">
-        <v>30</v>
+      <c r="B117" t="s">
+        <v>156</v>
       </c>
       <c r="C117" s="4">
         <v>31</v>
@@ -3079,8 +3222,8 @@
       <c r="A118" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B118" s="4" t="s">
-        <v>30</v>
+      <c r="B118" t="s">
+        <v>156</v>
       </c>
       <c r="C118" s="4">
         <v>31</v>
@@ -3093,14 +3236,301 @@
       <c r="A119" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B119" s="4" t="s">
-        <v>30</v>
+      <c r="B119" t="s">
+        <v>156</v>
       </c>
       <c r="C119" s="4">
         <v>31</v>
       </c>
       <c r="E119" s="4" t="s">
         <v>132</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A120" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B120" t="s">
+        <v>30</v>
+      </c>
+      <c r="C120" s="4">
+        <v>32</v>
+      </c>
+      <c r="E120" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="F120" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A121" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B121" t="s">
+        <v>30</v>
+      </c>
+      <c r="C121" s="4">
+        <v>32</v>
+      </c>
+      <c r="E121" s="4" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A122" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B122" t="s">
+        <v>30</v>
+      </c>
+      <c r="C122" s="4">
+        <v>32</v>
+      </c>
+      <c r="E122" s="4" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A123" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B123" t="s">
+        <v>30</v>
+      </c>
+      <c r="C123" s="4">
+        <v>33</v>
+      </c>
+      <c r="E123" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="F123" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A124" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B124" t="s">
+        <v>30</v>
+      </c>
+      <c r="C124" s="4">
+        <v>33</v>
+      </c>
+      <c r="E124" s="4" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A125" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B125" t="s">
+        <v>30</v>
+      </c>
+      <c r="C125" s="4">
+        <v>33</v>
+      </c>
+      <c r="E125" s="4" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A126" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B126" t="s">
+        <v>30</v>
+      </c>
+      <c r="C126" s="4">
+        <v>33</v>
+      </c>
+      <c r="E126" s="4" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A127" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B127" t="s">
+        <v>30</v>
+      </c>
+      <c r="C127" s="4">
+        <v>34</v>
+      </c>
+      <c r="E127" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="F127" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A128" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B128" t="s">
+        <v>30</v>
+      </c>
+      <c r="C128" s="4">
+        <v>34</v>
+      </c>
+      <c r="E128" s="4" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A129" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B129" t="s">
+        <v>30</v>
+      </c>
+      <c r="C129" s="4">
+        <v>34</v>
+      </c>
+      <c r="E129" s="4" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A130" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B130" t="s">
+        <v>30</v>
+      </c>
+      <c r="C130" s="4">
+        <v>34</v>
+      </c>
+      <c r="E130" s="4" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A131" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B131" t="s">
+        <v>30</v>
+      </c>
+      <c r="C131" s="4">
+        <v>35</v>
+      </c>
+      <c r="E131" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="F131" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A132" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B132" t="s">
+        <v>30</v>
+      </c>
+      <c r="C132" s="4">
+        <v>35</v>
+      </c>
+      <c r="E132" s="4" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A133" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B133" t="s">
+        <v>30</v>
+      </c>
+      <c r="C133" s="4">
+        <v>35</v>
+      </c>
+      <c r="E133" s="4" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A134" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B134" t="s">
+        <v>30</v>
+      </c>
+      <c r="C134" s="4">
+        <v>35</v>
+      </c>
+      <c r="E134" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A135" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B135" t="s">
+        <v>30</v>
+      </c>
+      <c r="C135" s="4">
+        <v>36</v>
+      </c>
+      <c r="E135" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="F135" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A136" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B136" t="s">
+        <v>30</v>
+      </c>
+      <c r="C136" s="4">
+        <v>36</v>
+      </c>
+      <c r="E136" s="4" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A137" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B137" t="s">
+        <v>30</v>
+      </c>
+      <c r="C137" s="4">
+        <v>36</v>
+      </c>
+      <c r="E137" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="F137" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A138" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B138" t="s">
+        <v>30</v>
+      </c>
+      <c r="C138" s="4">
+        <v>36</v>
+      </c>
+      <c r="E138" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="F138" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>